<commit_message>
Update 0.2 and added changelog
</commit_message>
<xml_diff>
--- a/mods.xlsx
+++ b/mods.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\KSP_win64\GameData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\GPTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A5F1F3-9BEF-4EE9-9288-E15FCD5AFEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD19CBC-6D59-4B4D-B81D-55C8AE818D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="756" windowWidth="23040" windowHeight="11604" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="241">
   <si>
     <t>USI Sounding Rockets</t>
   </si>
@@ -735,6 +735,30 @@
   </si>
   <si>
     <t>Another workshop/extraplanetary construction option</t>
+  </si>
+  <si>
+    <t>Knes</t>
+  </si>
+  <si>
+    <t>1.9.9</t>
+  </si>
+  <si>
+    <t>https://github.com/AstroWell/Knes/releases</t>
+  </si>
+  <si>
+    <t>Completely NonAggressive Rocketry</t>
+  </si>
+  <si>
+    <t>1.0.3</t>
+  </si>
+  <si>
+    <t>https://github.com/DylanSemrau/CompletelyNonAggressiveRocketry/releases</t>
+  </si>
+  <si>
+    <t>Mostly works quite well with some good early rockets, but a few odd parts; overpowered rcs units placed in Electric Engine Concepts on the logic that we could imagine they're resistojets?</t>
+  </si>
+  <si>
+    <t>Provides some good early rockets, though the command parts don't quite fit.</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1091,7 @@
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D88" sqref="C82:D88"/>
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1963,8 +1987,33 @@
         <v>232</v>
       </c>
     </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>233</v>
+      </c>
+      <c r="B72" t="s">
+        <v>234</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D72" t="s">
+        <v>239</v>
+      </c>
+    </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C73" s="2"/>
+      <c r="A73" t="s">
+        <v>236</v>
+      </c>
+      <c r="B73" t="s">
+        <v>237</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D73" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C91" s="2"/>
@@ -2046,6 +2095,8 @@
     <hyperlink ref="C30" r:id="rId61" xr:uid="{73F384B8-A259-468E-998F-F8B8793D348A}"/>
     <hyperlink ref="C70" r:id="rId62" xr:uid="{1BFFE1AC-A674-4F72-BFC7-867119D838A9}"/>
     <hyperlink ref="C71" r:id="rId63" xr:uid="{7A7261F3-7FE5-4937-A8E4-70A10A8F0DB7}"/>
+    <hyperlink ref="C72" r:id="rId64" xr:uid="{2A772898-BC4E-4F6C-89D0-B4B02B9514F6}"/>
+    <hyperlink ref="C73" r:id="rId65" xr:uid="{85CA4870-4CA2-4642-9C15-C46CFFA0B519}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>